<commit_message>
Rename Group script and update lecture slides
Renamed the 'Group' script from Lec_7 to Lec_8 and updated the Lec_7_8.xlsx slides to reflect changes for the new lecture.
</commit_message>
<xml_diff>
--- a/Beginner/Slides/Lec_7_8.xlsx
+++ b/Beginner/Slides/Lec_7_8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaotingzhou/Documents/Lectures/SQL/Beginner/Slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B53D904-66D1-E64B-8C7C-F23BD9F9971F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237B23B1-486E-9E44-A7EC-CE1A40159209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="6" xr2:uid="{B01DC677-87C8-C645-902B-49FC9EAA203F}"/>
   </bookViews>
@@ -3362,7 +3362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3478,6 +3478,16 @@
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3502,17 +3512,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4837,7 +4836,7 @@
       <c r="C28" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="71" t="s">
+      <c r="D28" s="81" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4851,7 +4850,7 @@
       <c r="C29" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="71"/>
+      <c r="D29" s="81"/>
     </row>
     <row r="30" spans="1:7" ht="30">
       <c r="A30" s="10" t="s">
@@ -4863,7 +4862,7 @@
       <c r="C30" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="71"/>
+      <c r="D30" s="81"/>
     </row>
     <row r="31" spans="1:7" ht="30">
       <c r="A31" s="10" t="s">
@@ -4875,7 +4874,7 @@
       <c r="C31" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="71"/>
+      <c r="D31" s="81"/>
     </row>
     <row r="32" spans="1:7" ht="30">
       <c r="A32" s="10" t="s">
@@ -4887,7 +4886,7 @@
       <c r="C32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="71"/>
+      <c r="D32" s="81"/>
     </row>
     <row r="33" spans="1:4" ht="30">
       <c r="A33" s="10" t="s">
@@ -4899,7 +4898,7 @@
       <c r="C33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="71"/>
+      <c r="D33" s="81"/>
     </row>
     <row r="34" spans="1:4" ht="30">
       <c r="A34" s="10" t="s">
@@ -4911,7 +4910,7 @@
       <c r="C34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="71"/>
+      <c r="D34" s="81"/>
     </row>
     <row r="35" spans="1:4" ht="30">
       <c r="A35" s="10" t="s">
@@ -4923,7 +4922,7 @@
       <c r="C35" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="71"/>
+      <c r="D35" s="81"/>
     </row>
     <row r="36" spans="1:4" ht="30">
       <c r="A36" s="10" t="s">
@@ -4935,7 +4934,7 @@
       <c r="C36" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="71"/>
+      <c r="D36" s="81"/>
     </row>
     <row r="37" spans="1:4" ht="30">
       <c r="A37" s="10" t="s">
@@ -4947,7 +4946,7 @@
       <c r="C37" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="71"/>
+      <c r="D37" s="81"/>
     </row>
     <row r="38" spans="1:4" ht="30">
       <c r="A38" s="10" t="s">
@@ -4959,7 +4958,7 @@
       <c r="C38" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="71"/>
+      <c r="D38" s="81"/>
     </row>
     <row r="39" spans="1:4" ht="30">
       <c r="A39" s="10" t="s">
@@ -4971,7 +4970,7 @@
       <c r="C39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="71"/>
+      <c r="D39" s="81"/>
     </row>
     <row r="40" spans="1:4" ht="30">
       <c r="A40" s="10" t="s">
@@ -4983,7 +4982,7 @@
       <c r="C40" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="71"/>
+      <c r="D40" s="81"/>
     </row>
     <row r="41" spans="1:4" ht="30">
       <c r="A41" s="10" t="s">
@@ -4995,7 +4994,7 @@
       <c r="C41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="71"/>
+      <c r="D41" s="81"/>
     </row>
     <row r="42" spans="1:4" ht="30">
       <c r="A42" s="10" t="s">
@@ -5007,7 +5006,7 @@
       <c r="C42" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="71"/>
+      <c r="D42" s="81"/>
     </row>
     <row r="43" spans="1:4" ht="30">
       <c r="A43" s="10" t="s">
@@ -5019,7 +5018,7 @@
       <c r="C43" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="71"/>
+      <c r="D43" s="81"/>
     </row>
     <row r="44" spans="1:4" ht="30">
       <c r="A44" s="10" t="s">
@@ -5031,7 +5030,7 @@
       <c r="C44" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="71"/>
+      <c r="D44" s="81"/>
     </row>
     <row r="52" spans="1:5" ht="27">
       <c r="A52" s="3" t="s">
@@ -5099,12 +5098,12 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="23">
-      <c r="A62" s="79" t="s">
+      <c r="A62" s="71" t="s">
         <v>871</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="23">
-      <c r="A63" s="79" t="s">
+      <c r="A63" s="71" t="s">
         <v>872</v>
       </c>
       <c r="B63" s="42"/>
@@ -5413,10 +5412,10 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="C46" s="72" t="s">
+      <c r="C46" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="D46" s="72"/>
+      <c r="D46" s="82"/>
     </row>
     <row r="47" spans="1:4">
       <c r="B47" s="22" t="s">
@@ -5636,7 +5635,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="86" t="s">
         <v>200</v>
       </c>
       <c r="C16" s="26" t="s">
@@ -5650,7 +5649,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="B17" s="77"/>
+      <c r="B17" s="87"/>
       <c r="C17" s="58" t="s">
         <v>485</v>
       </c>
@@ -5662,7 +5661,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="86" t="s">
         <v>205</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -5676,7 +5675,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="B19" s="77"/>
+      <c r="B19" s="87"/>
       <c r="C19" s="26" t="s">
         <v>209</v>
       </c>
@@ -5688,7 +5687,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="86" t="s">
         <v>212</v>
       </c>
       <c r="C20" s="26" t="s">
@@ -5702,7 +5701,7 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="B21" s="77"/>
+      <c r="B21" s="87"/>
       <c r="C21" s="26" t="s">
         <v>216</v>
       </c>
@@ -5742,7 +5741,7 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="86" t="s">
         <v>227</v>
       </c>
       <c r="C24" s="26" t="s">
@@ -5756,7 +5755,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="B25" s="78"/>
+      <c r="B25" s="88"/>
       <c r="C25" s="26" t="s">
         <v>229</v>
       </c>
@@ -5768,7 +5767,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="B26" s="77"/>
+      <c r="B26" s="87"/>
       <c r="C26" s="26" t="s">
         <v>232</v>
       </c>
@@ -5808,7 +5807,7 @@
       </c>
     </row>
     <row r="35" spans="2:12">
-      <c r="B35" s="73" t="s">
+      <c r="B35" s="83" t="s">
         <v>240</v>
       </c>
       <c r="C35" s="26" t="s">
@@ -5822,7 +5821,7 @@
       </c>
     </row>
     <row r="36" spans="2:12">
-      <c r="B36" s="74"/>
+      <c r="B36" s="84"/>
       <c r="C36" s="26" t="s">
         <v>243</v>
       </c>
@@ -5834,7 +5833,7 @@
       </c>
     </row>
     <row r="37" spans="2:12">
-      <c r="B37" s="74"/>
+      <c r="B37" s="84"/>
       <c r="C37" s="26" t="s">
         <v>604</v>
       </c>
@@ -5846,7 +5845,7 @@
       </c>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" s="74"/>
+      <c r="B38" s="84"/>
       <c r="C38" s="26" t="s">
         <v>248</v>
       </c>
@@ -5858,7 +5857,7 @@
       </c>
     </row>
     <row r="39" spans="2:12">
-      <c r="B39" s="74"/>
+      <c r="B39" s="84"/>
       <c r="C39" s="26" t="s">
         <v>250</v>
       </c>
@@ -5870,7 +5869,7 @@
       </c>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="75"/>
+      <c r="B40" s="85"/>
       <c r="C40" s="26" t="s">
         <v>252</v>
       </c>
@@ -5882,7 +5881,7 @@
       </c>
     </row>
     <row r="41" spans="2:12">
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="83" t="s">
         <v>255</v>
       </c>
       <c r="C41" s="26" t="s">
@@ -5896,7 +5895,7 @@
       </c>
     </row>
     <row r="42" spans="2:12">
-      <c r="B42" s="74"/>
+      <c r="B42" s="84"/>
       <c r="C42" s="26" t="s">
         <v>259</v>
       </c>
@@ -5908,7 +5907,7 @@
       </c>
     </row>
     <row r="43" spans="2:12">
-      <c r="B43" s="74"/>
+      <c r="B43" s="84"/>
       <c r="C43" s="59" t="s">
         <v>606</v>
       </c>
@@ -5923,7 +5922,7 @@
       </c>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="74"/>
+      <c r="B44" s="84"/>
       <c r="C44" s="26" t="s">
         <v>605</v>
       </c>
@@ -5935,7 +5934,7 @@
       </c>
     </row>
     <row r="45" spans="2:12">
-      <c r="B45" s="74"/>
+      <c r="B45" s="84"/>
       <c r="C45" s="26" t="s">
         <v>264</v>
       </c>
@@ -5950,7 +5949,7 @@
       </c>
     </row>
     <row r="46" spans="2:12">
-      <c r="B46" s="75"/>
+      <c r="B46" s="85"/>
       <c r="C46" s="26" t="s">
         <v>266</v>
       </c>
@@ -5963,10 +5962,10 @@
       <c r="L46" s="46"/>
     </row>
     <row r="47" spans="2:12">
-      <c r="B47" s="73" t="s">
+      <c r="B47" s="83" t="s">
         <v>268</v>
       </c>
-      <c r="C47" s="85" t="s">
+      <c r="C47" s="26" t="s">
         <v>269</v>
       </c>
       <c r="D47" s="26" t="s">
@@ -5980,8 +5979,8 @@
       </c>
     </row>
     <row r="48" spans="2:12">
-      <c r="B48" s="74"/>
-      <c r="C48" s="85" t="s">
+      <c r="B48" s="84"/>
+      <c r="C48" s="26" t="s">
         <v>272</v>
       </c>
       <c r="D48" s="26" t="s">
@@ -5993,8 +5992,8 @@
       <c r="L48" s="46"/>
     </row>
     <row r="49" spans="2:12">
-      <c r="B49" s="74"/>
-      <c r="C49" s="85" t="s">
+      <c r="B49" s="84"/>
+      <c r="C49" s="26" t="s">
         <v>275</v>
       </c>
       <c r="D49" s="26" t="s">
@@ -6008,8 +6007,8 @@
       </c>
     </row>
     <row r="50" spans="2:12">
-      <c r="B50" s="74"/>
-      <c r="C50" s="85" t="s">
+      <c r="B50" s="84"/>
+      <c r="C50" s="26" t="s">
         <v>278</v>
       </c>
       <c r="D50" s="26" t="s">
@@ -6021,8 +6020,8 @@
       <c r="L50" s="46"/>
     </row>
     <row r="51" spans="2:12">
-      <c r="B51" s="74"/>
-      <c r="C51" s="85" t="s">
+      <c r="B51" s="84"/>
+      <c r="C51" s="26" t="s">
         <v>281</v>
       </c>
       <c r="D51" s="26" t="s">
@@ -6036,8 +6035,8 @@
       </c>
     </row>
     <row r="52" spans="2:12">
-      <c r="B52" s="75"/>
-      <c r="C52" s="85" t="s">
+      <c r="B52" s="85"/>
+      <c r="C52" s="26" t="s">
         <v>284</v>
       </c>
       <c r="D52" s="26" t="s">
@@ -6048,7 +6047,7 @@
       </c>
     </row>
     <row r="53" spans="2:12">
-      <c r="B53" s="73" t="s">
+      <c r="B53" s="83" t="s">
         <v>287</v>
       </c>
       <c r="C53" s="48" t="s">
@@ -6062,7 +6061,7 @@
       </c>
     </row>
     <row r="54" spans="2:12">
-      <c r="B54" s="74"/>
+      <c r="B54" s="84"/>
       <c r="C54" s="48" t="s">
         <v>291</v>
       </c>
@@ -6074,7 +6073,7 @@
       </c>
     </row>
     <row r="55" spans="2:12">
-      <c r="B55" s="74"/>
+      <c r="B55" s="84"/>
       <c r="C55" s="48" t="s">
         <v>294</v>
       </c>
@@ -6086,7 +6085,7 @@
       </c>
     </row>
     <row r="56" spans="2:12">
-      <c r="B56" s="74"/>
+      <c r="B56" s="84"/>
       <c r="C56" s="48" t="s">
         <v>297</v>
       </c>
@@ -6098,19 +6097,19 @@
       </c>
     </row>
     <row r="57" spans="2:12">
-      <c r="B57" s="75"/>
+      <c r="B57" s="85"/>
       <c r="C57" s="48" t="s">
         <v>300</v>
       </c>
       <c r="D57" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="E57" s="86" t="s">
+      <c r="E57" s="77" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="58" spans="2:12">
-      <c r="B58" s="73" t="s">
+      <c r="B58" s="83" t="s">
         <v>303</v>
       </c>
       <c r="C58" s="26" t="s">
@@ -6124,7 +6123,7 @@
       </c>
     </row>
     <row r="59" spans="2:12">
-      <c r="B59" s="74"/>
+      <c r="B59" s="84"/>
       <c r="C59" s="26" t="s">
         <v>307</v>
       </c>
@@ -6136,7 +6135,7 @@
       </c>
     </row>
     <row r="60" spans="2:12">
-      <c r="B60" s="74"/>
+      <c r="B60" s="84"/>
       <c r="C60" s="26" t="s">
         <v>310</v>
       </c>
@@ -6148,7 +6147,7 @@
       </c>
     </row>
     <row r="61" spans="2:12">
-      <c r="B61" s="75"/>
+      <c r="B61" s="85"/>
       <c r="C61" s="26" t="s">
         <v>313</v>
       </c>
@@ -9126,7 +9125,7 @@
       <c r="G1" s="69" t="s">
         <v>873</v>
       </c>
-      <c r="H1" s="83"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="64">
@@ -9148,7 +9147,7 @@
         <v>291</v>
       </c>
       <c r="G2" s="70"/>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="76" t="s">
         <v>874</v>
       </c>
     </row>
@@ -9172,7 +9171,7 @@
         <v>294</v>
       </c>
       <c r="G3" s="65"/>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="76" t="s">
         <v>630</v>
       </c>
     </row>
@@ -9192,7 +9191,7 @@
         <v>297</v>
       </c>
       <c r="G4" s="65"/>
-      <c r="H4" s="84" t="s">
+      <c r="H4" s="76" t="s">
         <v>813</v>
       </c>
     </row>
@@ -9214,7 +9213,7 @@
         <v>300</v>
       </c>
       <c r="G5" s="65"/>
-      <c r="H5" s="83"/>
+      <c r="H5" s="75"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="64">
@@ -9233,7 +9232,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="70"/>
-      <c r="H6" s="83"/>
+      <c r="H6" s="75"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="64">
@@ -9251,11 +9250,11 @@
       <c r="E7" s="64">
         <v>2</v>
       </c>
-      <c r="F7" s="89"/>
+      <c r="F7" s="80"/>
       <c r="G7" s="69" t="s">
         <v>814</v>
       </c>
-      <c r="H7" s="87"/>
+      <c r="H7" s="78"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="64">
@@ -9274,7 +9273,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="70"/>
-      <c r="H8" s="88" t="s">
+      <c r="H8" s="79" t="s">
         <v>815</v>
       </c>
     </row>
@@ -9293,7 +9292,7 @@
       </c>
       <c r="E9" s="64"/>
       <c r="G9" s="65"/>
-      <c r="H9" s="88" t="s">
+      <c r="H9" s="79" t="s">
         <v>630</v>
       </c>
     </row>
@@ -9313,9 +9312,9 @@
       <c r="E10" s="64">
         <v>2</v>
       </c>
-      <c r="F10" s="87"/>
+      <c r="F10" s="78"/>
       <c r="G10" s="65"/>
-      <c r="H10" s="88" t="s">
+      <c r="H10" s="79" t="s">
         <v>816</v>
       </c>
     </row>
@@ -9336,7 +9335,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="65"/>
-      <c r="H11" s="87"/>
+      <c r="H11" s="78"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="64">
@@ -9353,7 +9352,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="70"/>
-      <c r="H12" s="87"/>
+      <c r="H12" s="78"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="64">
@@ -10529,742 +10528,742 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:5" ht="24">
-      <c r="A1" s="80">
+      <c r="A1" s="72">
         <v>3001</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="72" t="s">
         <v>761</v>
       </c>
-      <c r="C1" s="80">
+      <c r="C1" s="72">
         <v>20</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="72" t="s">
         <v>762</v>
       </c>
-      <c r="E1" s="80">
+      <c r="E1" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="24">
-      <c r="A2" s="80">
+      <c r="A2" s="72">
         <v>3005</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="72" t="s">
         <v>766</v>
       </c>
-      <c r="C2" s="80">
+      <c r="C2" s="72">
         <v>19</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D2" s="72" t="s">
         <v>762</v>
       </c>
-      <c r="E2" s="80">
+      <c r="E2" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="24">
-      <c r="A3" s="80">
+      <c r="A3" s="72">
         <v>3010</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="72" t="s">
         <v>771</v>
       </c>
-      <c r="C3" s="80">
+      <c r="C3" s="72">
         <v>22</v>
       </c>
-      <c r="D3" s="80" t="s">
+      <c r="D3" s="72" t="s">
         <v>764</v>
       </c>
-      <c r="E3" s="80">
+      <c r="E3" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="24">
-      <c r="A4" s="80">
+      <c r="A4" s="72">
         <v>3012</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="72" t="s">
         <v>773</v>
       </c>
-      <c r="C4" s="80">
+      <c r="C4" s="72">
         <v>25</v>
       </c>
-      <c r="D4" s="80" t="s">
+      <c r="D4" s="72" t="s">
         <v>764</v>
       </c>
-      <c r="E4" s="80">
+      <c r="E4" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24">
-      <c r="A5" s="80">
+      <c r="A5" s="72">
         <v>3015</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="72" t="s">
         <v>776</v>
       </c>
-      <c r="C5" s="80">
+      <c r="C5" s="72">
         <v>21</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="72" t="s">
         <v>762</v>
       </c>
-      <c r="E5" s="80">
+      <c r="E5" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="24">
-      <c r="A6" s="80">
+      <c r="A6" s="72">
         <v>3017</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="72" t="s">
         <v>778</v>
       </c>
-      <c r="C6" s="80">
+      <c r="C6" s="72">
         <v>22</v>
       </c>
-      <c r="D6" s="80" t="s">
+      <c r="D6" s="72" t="s">
         <v>762</v>
       </c>
-      <c r="E6" s="80">
+      <c r="E6" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="24">
-      <c r="A7" s="80">
+      <c r="A7" s="72">
         <v>3021</v>
       </c>
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="72" t="s">
         <v>783</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80" t="s">
+      <c r="C7" s="72"/>
+      <c r="D7" s="72" t="s">
         <v>762</v>
       </c>
-      <c r="E7" s="80">
+      <c r="E7" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="24">
-      <c r="A8" s="80">
+      <c r="A8" s="72">
         <v>3024</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="72" t="s">
         <v>786</v>
       </c>
-      <c r="C8" s="80">
+      <c r="C8" s="72">
         <v>22</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="72" t="s">
         <v>762</v>
       </c>
-      <c r="E8" s="80">
+      <c r="E8" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24">
-      <c r="A9" s="80">
+      <c r="A9" s="72">
         <v>3027</v>
       </c>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="72" t="s">
         <v>789</v>
       </c>
-      <c r="C9" s="80">
+      <c r="C9" s="72">
         <v>25</v>
       </c>
-      <c r="D9" s="80" t="s">
+      <c r="D9" s="72" t="s">
         <v>764</v>
       </c>
-      <c r="E9" s="80">
+      <c r="E9" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="24">
-      <c r="A10" s="80">
+      <c r="A10" s="72">
         <v>3030</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="72" t="s">
         <v>792</v>
       </c>
-      <c r="C10" s="80">
+      <c r="C10" s="72">
         <v>18</v>
       </c>
-      <c r="D10" s="80" t="s">
+      <c r="D10" s="72" t="s">
         <v>762</v>
       </c>
-      <c r="E10" s="80">
+      <c r="E10" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="24">
-      <c r="A11" s="80">
+      <c r="A11" s="72">
         <v>3033</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="72" t="s">
         <v>795</v>
       </c>
-      <c r="C11" s="80">
+      <c r="C11" s="72">
         <v>28</v>
       </c>
-      <c r="D11" s="80" t="s">
+      <c r="D11" s="72" t="s">
         <v>764</v>
       </c>
-      <c r="E11" s="80">
+      <c r="E11" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="24">
-      <c r="A12" s="80">
+      <c r="A12" s="72">
         <v>3038</v>
       </c>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="72" t="s">
         <v>800</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80" t="s">
+      <c r="C12" s="72"/>
+      <c r="D12" s="72" t="s">
         <v>762</v>
       </c>
-      <c r="E12" s="80">
+      <c r="E12" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="24">
-      <c r="A13" s="80">
+      <c r="A13" s="72">
         <v>3040</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="72" t="s">
         <v>802</v>
       </c>
-      <c r="C13" s="80">
+      <c r="C13" s="72">
         <v>20</v>
       </c>
-      <c r="D13" s="80" t="s">
+      <c r="D13" s="72" t="s">
         <v>762</v>
       </c>
-      <c r="E13" s="80">
+      <c r="E13" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="24">
-      <c r="A14" s="80">
+      <c r="A14" s="72">
         <v>3043</v>
       </c>
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="72" t="s">
         <v>805</v>
       </c>
-      <c r="C14" s="80">
+      <c r="C14" s="72">
         <v>26</v>
       </c>
-      <c r="D14" s="80" t="s">
+      <c r="D14" s="72" t="s">
         <v>764</v>
       </c>
-      <c r="E14" s="80">
+      <c r="E14" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="24">
-      <c r="A15" s="80">
+      <c r="A15" s="72">
         <v>3045</v>
       </c>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="72" t="s">
         <v>807</v>
       </c>
-      <c r="C15" s="80">
+      <c r="C15" s="72">
         <v>20</v>
       </c>
-      <c r="D15" s="80" t="s">
+      <c r="D15" s="72" t="s">
         <v>764</v>
       </c>
-      <c r="E15" s="80">
+      <c r="E15" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="24">
-      <c r="A16" s="80">
+      <c r="A16" s="72">
         <v>3049</v>
       </c>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="72" t="s">
         <v>811</v>
       </c>
-      <c r="C16" s="80">
+      <c r="C16" s="72">
         <v>23</v>
       </c>
-      <c r="D16" s="80" t="s">
+      <c r="D16" s="72" t="s">
         <v>764</v>
       </c>
-      <c r="E16" s="80">
+      <c r="E16" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="24">
-      <c r="A17" s="81">
+      <c r="A17" s="73">
         <v>3002</v>
       </c>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="73" t="s">
         <v>763</v>
       </c>
-      <c r="C17" s="81">
+      <c r="C17" s="73">
         <v>21</v>
       </c>
-      <c r="D17" s="81" t="s">
+      <c r="D17" s="73" t="s">
         <v>764</v>
       </c>
-      <c r="E17" s="81">
+      <c r="E17" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="24">
-      <c r="A18" s="81">
+      <c r="A18" s="73">
         <v>3006</v>
       </c>
-      <c r="B18" s="81" t="s">
+      <c r="B18" s="73" t="s">
         <v>767</v>
       </c>
-      <c r="C18" s="81">
+      <c r="C18" s="73">
         <v>24</v>
       </c>
-      <c r="D18" s="81" t="s">
+      <c r="D18" s="73" t="s">
         <v>764</v>
       </c>
-      <c r="E18" s="81">
+      <c r="E18" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="24">
-      <c r="A19" s="81">
+      <c r="A19" s="73">
         <v>3009</v>
       </c>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="73" t="s">
         <v>770</v>
       </c>
-      <c r="C19" s="81">
+      <c r="C19" s="73">
         <v>20</v>
       </c>
-      <c r="D19" s="81" t="s">
+      <c r="D19" s="73" t="s">
         <v>762</v>
       </c>
-      <c r="E19" s="81">
+      <c r="E19" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="24">
-      <c r="A20" s="81">
+      <c r="A20" s="73">
         <v>3013</v>
       </c>
-      <c r="B20" s="81" t="s">
+      <c r="B20" s="73" t="s">
         <v>774</v>
       </c>
-      <c r="C20" s="81">
+      <c r="C20" s="73">
         <v>20</v>
       </c>
-      <c r="D20" s="81" t="s">
+      <c r="D20" s="73" t="s">
         <v>762</v>
       </c>
-      <c r="E20" s="81">
+      <c r="E20" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="24">
-      <c r="A21" s="81">
+      <c r="A21" s="73">
         <v>3016</v>
       </c>
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="73" t="s">
         <v>777</v>
       </c>
-      <c r="C21" s="81">
+      <c r="C21" s="73">
         <v>30</v>
       </c>
-      <c r="D21" s="81" t="s">
+      <c r="D21" s="73" t="s">
         <v>764</v>
       </c>
-      <c r="E21" s="81">
+      <c r="E21" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="24">
-      <c r="A22" s="81">
+      <c r="A22" s="73">
         <v>3018</v>
       </c>
-      <c r="B22" s="81" t="s">
+      <c r="B22" s="73" t="s">
         <v>779</v>
       </c>
-      <c r="C22" s="81">
+      <c r="C22" s="73">
         <v>23</v>
       </c>
-      <c r="D22" s="81" t="s">
+      <c r="D22" s="73" t="s">
         <v>780</v>
       </c>
-      <c r="E22" s="81">
+      <c r="E22" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="24">
-      <c r="A23" s="81">
+      <c r="A23" s="73">
         <v>3022</v>
       </c>
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="73" t="s">
         <v>784</v>
       </c>
-      <c r="C23" s="81">
+      <c r="C23" s="73">
         <v>20</v>
       </c>
-      <c r="D23" s="81" t="s">
+      <c r="D23" s="73" t="s">
         <v>762</v>
       </c>
-      <c r="E23" s="81">
+      <c r="E23" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="24">
-      <c r="A24" s="81">
+      <c r="A24" s="73">
         <v>3025</v>
       </c>
-      <c r="B24" s="81" t="s">
+      <c r="B24" s="73" t="s">
         <v>787</v>
       </c>
-      <c r="C24" s="81">
+      <c r="C24" s="73">
         <v>20</v>
       </c>
-      <c r="D24" s="81" t="s">
+      <c r="D24" s="73" t="s">
         <v>764</v>
       </c>
-      <c r="E24" s="81">
+      <c r="E24" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="24">
-      <c r="A25" s="81">
+      <c r="A25" s="73">
         <v>3029</v>
       </c>
-      <c r="B25" s="81" t="s">
+      <c r="B25" s="73" t="s">
         <v>791</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="73">
         <v>24</v>
       </c>
-      <c r="D25" s="81" t="s">
+      <c r="D25" s="73" t="s">
         <v>764</v>
       </c>
-      <c r="E25" s="81">
+      <c r="E25" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="24">
-      <c r="A26" s="81">
+      <c r="A26" s="73">
         <v>3032</v>
       </c>
-      <c r="B26" s="81" t="s">
+      <c r="B26" s="73" t="s">
         <v>794</v>
       </c>
-      <c r="C26" s="81">
+      <c r="C26" s="73">
         <v>19</v>
       </c>
-      <c r="D26" s="81" t="s">
+      <c r="D26" s="73" t="s">
         <v>762</v>
       </c>
-      <c r="E26" s="81">
+      <c r="E26" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="24">
-      <c r="A27" s="81">
+      <c r="A27" s="73">
         <v>3036</v>
       </c>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="73" t="s">
         <v>798</v>
       </c>
-      <c r="C27" s="81">
+      <c r="C27" s="73">
         <v>20</v>
       </c>
-      <c r="D27" s="81" t="s">
+      <c r="D27" s="73" t="s">
         <v>762</v>
       </c>
-      <c r="E27" s="81">
+      <c r="E27" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="24">
-      <c r="A28" s="81">
+      <c r="A28" s="73">
         <v>3039</v>
       </c>
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="73" t="s">
         <v>801</v>
       </c>
-      <c r="C28" s="81">
+      <c r="C28" s="73">
         <v>21</v>
       </c>
-      <c r="D28" s="81" t="s">
+      <c r="D28" s="73" t="s">
         <v>764</v>
       </c>
-      <c r="E28" s="81">
+      <c r="E28" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="24">
-      <c r="A29" s="81">
+      <c r="A29" s="73">
         <v>3042</v>
       </c>
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="73" t="s">
         <v>804</v>
       </c>
-      <c r="C29" s="81">
+      <c r="C29" s="73">
         <v>24</v>
       </c>
-      <c r="D29" s="81" t="s">
+      <c r="D29" s="73" t="s">
         <v>762</v>
       </c>
-      <c r="E29" s="81">
+      <c r="E29" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="24">
-      <c r="A30" s="81">
+      <c r="A30" s="73">
         <v>3046</v>
       </c>
-      <c r="B30" s="81" t="s">
+      <c r="B30" s="73" t="s">
         <v>808</v>
       </c>
-      <c r="C30" s="81">
+      <c r="C30" s="73">
         <v>19</v>
       </c>
-      <c r="D30" s="81" t="s">
+      <c r="D30" s="73" t="s">
         <v>762</v>
       </c>
-      <c r="E30" s="81">
+      <c r="E30" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="24">
-      <c r="A31" s="81">
+      <c r="A31" s="73">
         <v>3050</v>
       </c>
-      <c r="B31" s="81" t="s">
+      <c r="B31" s="73" t="s">
         <v>812</v>
       </c>
-      <c r="C31" s="81">
+      <c r="C31" s="73">
         <v>21</v>
       </c>
-      <c r="D31" s="81" t="s">
+      <c r="D31" s="73" t="s">
         <v>762</v>
       </c>
-      <c r="E31" s="81">
+      <c r="E31" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="24">
-      <c r="A32" s="82">
+      <c r="A32" s="74">
         <v>3004</v>
       </c>
-      <c r="B32" s="82"/>
-      <c r="C32" s="82">
+      <c r="B32" s="74"/>
+      <c r="C32" s="74">
         <v>22</v>
       </c>
-      <c r="D32" s="82" t="s">
+      <c r="D32" s="74" t="s">
         <v>762</v>
       </c>
-      <c r="E32" s="82">
+      <c r="E32" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="24">
-      <c r="A33" s="82">
+      <c r="A33" s="74">
         <v>3007</v>
       </c>
-      <c r="B33" s="82" t="s">
+      <c r="B33" s="74" t="s">
         <v>768</v>
       </c>
-      <c r="C33" s="82">
+      <c r="C33" s="74">
         <v>20</v>
       </c>
-      <c r="D33" s="82" t="s">
+      <c r="D33" s="74" t="s">
         <v>762</v>
       </c>
-      <c r="E33" s="82">
+      <c r="E33" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="24">
-      <c r="A34" s="82">
+      <c r="A34" s="74">
         <v>3011</v>
       </c>
-      <c r="B34" s="82" t="s">
+      <c r="B34" s="74" t="s">
         <v>772</v>
       </c>
-      <c r="C34" s="82"/>
-      <c r="D34" s="82" t="s">
+      <c r="C34" s="74"/>
+      <c r="D34" s="74" t="s">
         <v>762</v>
       </c>
-      <c r="E34" s="82">
+      <c r="E34" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="24">
-      <c r="A35" s="82">
+      <c r="A35" s="74">
         <v>3014</v>
       </c>
-      <c r="B35" s="82" t="s">
+      <c r="B35" s="74" t="s">
         <v>775</v>
       </c>
-      <c r="C35" s="82">
+      <c r="C35" s="74">
         <v>28</v>
       </c>
-      <c r="D35" s="82" t="s">
+      <c r="D35" s="74" t="s">
         <v>764</v>
       </c>
-      <c r="E35" s="82">
+      <c r="E35" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="24">
-      <c r="A36" s="82">
+      <c r="A36" s="74">
         <v>3020</v>
       </c>
-      <c r="B36" s="82" t="s">
+      <c r="B36" s="74" t="s">
         <v>782</v>
       </c>
-      <c r="C36" s="82">
+      <c r="C36" s="74">
         <v>19</v>
       </c>
-      <c r="D36" s="82" t="s">
+      <c r="D36" s="74" t="s">
         <v>764</v>
       </c>
-      <c r="E36" s="82">
+      <c r="E36" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="24">
-      <c r="A37" s="82">
+      <c r="A37" s="74">
         <v>3023</v>
       </c>
-      <c r="B37" s="82" t="s">
+      <c r="B37" s="74" t="s">
         <v>785</v>
       </c>
-      <c r="C37" s="82">
+      <c r="C37" s="74">
         <v>21</v>
       </c>
-      <c r="D37" s="82" t="s">
+      <c r="D37" s="74" t="s">
         <v>764</v>
       </c>
-      <c r="E37" s="82">
+      <c r="E37" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="24">
-      <c r="A38" s="82">
+      <c r="A38" s="74">
         <v>3026</v>
       </c>
-      <c r="B38" s="82" t="s">
+      <c r="B38" s="74" t="s">
         <v>788</v>
       </c>
-      <c r="C38" s="82">
+      <c r="C38" s="74">
         <v>23</v>
       </c>
-      <c r="D38" s="82" t="s">
+      <c r="D38" s="74" t="s">
         <v>762</v>
       </c>
-      <c r="E38" s="82">
+      <c r="E38" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="24">
-      <c r="A39" s="82">
+      <c r="A39" s="74">
         <v>3031</v>
       </c>
-      <c r="B39" s="82" t="s">
+      <c r="B39" s="74" t="s">
         <v>793</v>
       </c>
-      <c r="C39" s="82">
+      <c r="C39" s="74">
         <v>27</v>
       </c>
-      <c r="D39" s="82" t="s">
+      <c r="D39" s="74" t="s">
         <v>764</v>
       </c>
-      <c r="E39" s="82">
+      <c r="E39" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="24">
-      <c r="A40" s="82">
+      <c r="A40" s="74">
         <v>3034</v>
       </c>
-      <c r="B40" s="82" t="s">
+      <c r="B40" s="74" t="s">
         <v>796</v>
       </c>
-      <c r="C40" s="82">
+      <c r="C40" s="74">
         <v>21</v>
       </c>
-      <c r="D40" s="82" t="s">
+      <c r="D40" s="74" t="s">
         <v>762</v>
       </c>
-      <c r="E40" s="82">
+      <c r="E40" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="24">
-      <c r="A41" s="82">
+      <c r="A41" s="74">
         <v>3037</v>
       </c>
-      <c r="B41" s="82" t="s">
+      <c r="B41" s="74" t="s">
         <v>799</v>
       </c>
-      <c r="C41" s="82">
+      <c r="C41" s="74">
         <v>23</v>
       </c>
-      <c r="D41" s="82" t="s">
+      <c r="D41" s="74" t="s">
         <v>764</v>
       </c>
-      <c r="E41" s="82">
+      <c r="E41" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="24">
-      <c r="A42" s="82">
+      <c r="A42" s="74">
         <v>3041</v>
       </c>
-      <c r="B42" s="82" t="s">
+      <c r="B42" s="74" t="s">
         <v>803</v>
       </c>
-      <c r="C42" s="82">
+      <c r="C42" s="74">
         <v>29</v>
       </c>
-      <c r="D42" s="82" t="s">
+      <c r="D42" s="74" t="s">
         <v>764</v>
       </c>
-      <c r="E42" s="82">
+      <c r="E42" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="24">
-      <c r="A43" s="82">
+      <c r="A43" s="74">
         <v>3044</v>
       </c>
-      <c r="B43" s="82" t="s">
+      <c r="B43" s="74" t="s">
         <v>806</v>
       </c>
-      <c r="C43" s="82">
+      <c r="C43" s="74">
         <v>22</v>
       </c>
-      <c r="D43" s="82" t="s">
+      <c r="D43" s="74" t="s">
         <v>762</v>
       </c>
-      <c r="E43" s="82">
+      <c r="E43" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="24">
-      <c r="A44" s="82">
+      <c r="A44" s="74">
         <v>3048</v>
       </c>
-      <c r="B44" s="82" t="s">
+      <c r="B44" s="74" t="s">
         <v>810</v>
       </c>
-      <c r="C44" s="82">
+      <c r="C44" s="74">
         <v>28</v>
       </c>
-      <c r="D44" s="82" t="s">
+      <c r="D44" s="74" t="s">
         <v>762</v>
       </c>
-      <c r="E44" s="82">
+      <c r="E44" s="74">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add date/time SQL script and update lecture slides
Added a new SQL script 'Date_Intro' demonstrating date/time functions and queries for students and courses. Included a credit card dataset for projects and updated lecture slides for sessions 3-4, 5-6, and 7-8.
</commit_message>
<xml_diff>
--- a/Beginner/Slides/Lec_7_8.xlsx
+++ b/Beginner/Slides/Lec_7_8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaotingzhou/Documents/Lectures/SQL/Beginner/Slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F161F827-004A-4043-A2A7-455F7AEB1E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13889F4-236F-BC4E-B26D-644BF5301F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="10" xr2:uid="{B01DC677-87C8-C645-902B-49FC9EAA203F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="6" xr2:uid="{B01DC677-87C8-C645-902B-49FC9EAA203F}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL" sheetId="6" r:id="rId1"/>
@@ -5239,7 +5239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5362,6 +5362,34 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="59" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="68" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5386,35 +5414,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="59" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="68" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5536,8 +5535,8 @@
       <xdr:row>86</xdr:row>
       <xdr:rowOff>46506</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="23" name="Ink 22">
@@ -5556,7 +5555,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="23" name="Ink 22">
@@ -7022,7 +7021,7 @@
       <c r="C28" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="78" t="s">
+      <c r="D28" s="106" t="s">
         <v>93</v>
       </c>
     </row>
@@ -7036,7 +7035,7 @@
       <c r="C29" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="78"/>
+      <c r="D29" s="106"/>
     </row>
     <row r="30" spans="1:7" ht="30">
       <c r="A30" s="10" t="s">
@@ -7048,7 +7047,7 @@
       <c r="C30" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="78"/>
+      <c r="D30" s="106"/>
     </row>
     <row r="31" spans="1:7" ht="30">
       <c r="A31" s="10" t="s">
@@ -7060,7 +7059,7 @@
       <c r="C31" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="78"/>
+      <c r="D31" s="106"/>
     </row>
     <row r="32" spans="1:7" ht="30">
       <c r="A32" s="10" t="s">
@@ -7072,7 +7071,7 @@
       <c r="C32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="78"/>
+      <c r="D32" s="106"/>
     </row>
     <row r="33" spans="1:4" ht="30">
       <c r="A33" s="10" t="s">
@@ -7084,7 +7083,7 @@
       <c r="C33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="78"/>
+      <c r="D33" s="106"/>
     </row>
     <row r="34" spans="1:4" ht="30">
       <c r="A34" s="10" t="s">
@@ -7096,7 +7095,7 @@
       <c r="C34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="78"/>
+      <c r="D34" s="106"/>
     </row>
     <row r="35" spans="1:4" ht="30">
       <c r="A35" s="10" t="s">
@@ -7108,7 +7107,7 @@
       <c r="C35" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="78"/>
+      <c r="D35" s="106"/>
     </row>
     <row r="36" spans="1:4" ht="30">
       <c r="A36" s="10" t="s">
@@ -7120,7 +7119,7 @@
       <c r="C36" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="78"/>
+      <c r="D36" s="106"/>
     </row>
     <row r="37" spans="1:4" ht="30">
       <c r="A37" s="10" t="s">
@@ -7132,7 +7131,7 @@
       <c r="C37" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="78"/>
+      <c r="D37" s="106"/>
     </row>
     <row r="38" spans="1:4" ht="30">
       <c r="A38" s="10" t="s">
@@ -7144,7 +7143,7 @@
       <c r="C38" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="78"/>
+      <c r="D38" s="106"/>
     </row>
     <row r="39" spans="1:4" ht="30">
       <c r="A39" s="10" t="s">
@@ -7156,7 +7155,7 @@
       <c r="C39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="78"/>
+      <c r="D39" s="106"/>
     </row>
     <row r="40" spans="1:4" ht="30">
       <c r="A40" s="10" t="s">
@@ -7168,7 +7167,7 @@
       <c r="C40" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="78"/>
+      <c r="D40" s="106"/>
     </row>
     <row r="41" spans="1:4" ht="30">
       <c r="A41" s="10" t="s">
@@ -7180,7 +7179,7 @@
       <c r="C41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="78"/>
+      <c r="D41" s="106"/>
     </row>
     <row r="42" spans="1:4" ht="30">
       <c r="A42" s="10" t="s">
@@ -7192,7 +7191,7 @@
       <c r="C42" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="78"/>
+      <c r="D42" s="106"/>
     </row>
     <row r="43" spans="1:4" ht="30">
       <c r="A43" s="10" t="s">
@@ -7204,7 +7203,7 @@
       <c r="C43" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="78"/>
+      <c r="D43" s="106"/>
     </row>
     <row r="44" spans="1:4" ht="30">
       <c r="A44" s="10" t="s">
@@ -7216,7 +7215,7 @@
       <c r="C44" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="78"/>
+      <c r="D44" s="106"/>
     </row>
     <row r="52" spans="1:5" ht="27">
       <c r="A52" s="3" t="s">
@@ -7350,44 +7349,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="78" t="s">
         <v>960</v>
       </c>
-      <c r="L1" s="86" t="s">
+      <c r="L1" s="78" t="s">
         <v>988</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="91" t="s">
         <v>760</v>
       </c>
-      <c r="C2" s="99" t="s">
+      <c r="C2" s="91" t="s">
         <v>952</v>
       </c>
-      <c r="D2" s="99" t="s">
+      <c r="D2" s="91" t="s">
         <v>953</v>
       </c>
-      <c r="E2" s="99" t="s">
+      <c r="E2" s="91" t="s">
         <v>954</v>
       </c>
-      <c r="F2" s="99" t="s">
+      <c r="F2" s="91" t="s">
         <v>955</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="94">
+      <c r="B3" s="86">
         <v>1</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="86" t="s">
         <v>956</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="86" t="s">
         <v>957</v>
       </c>
-      <c r="E3" s="95">
+      <c r="E3" s="87">
         <v>45839.375</v>
       </c>
-      <c r="F3" s="94">
+      <c r="F3" s="86">
         <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -7395,19 +7394,19 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="94">
+      <c r="B4" s="86">
         <v>2</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="86" t="s">
         <v>958</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="86" t="s">
         <v>959</v>
       </c>
-      <c r="E4" s="95">
+      <c r="E4" s="87">
         <v>45839.375</v>
       </c>
-      <c r="F4" s="94">
+      <c r="F4" s="86">
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -7415,7 +7414,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="19">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="78" t="s">
         <v>961</v>
       </c>
       <c r="M7" s="15" t="s">
@@ -7423,22 +7422,22 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="17">
-      <c r="B8" s="99" t="s">
+      <c r="B8" s="91" t="s">
         <v>962</v>
       </c>
-      <c r="C8" s="99" t="s">
+      <c r="C8" s="91" t="s">
         <v>757</v>
       </c>
-      <c r="D8" s="99" t="s">
+      <c r="D8" s="91" t="s">
         <v>963</v>
       </c>
-      <c r="E8" s="99" t="s">
+      <c r="E8" s="91" t="s">
         <v>964</v>
       </c>
-      <c r="F8" s="99" t="s">
+      <c r="F8" s="91" t="s">
         <v>965</v>
       </c>
-      <c r="G8" s="99" t="s">
+      <c r="G8" s="91" t="s">
         <v>966</v>
       </c>
       <c r="M8" s="15" t="s">
@@ -7446,22 +7445,22 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="17">
-      <c r="B9" s="94">
+      <c r="B9" s="86">
         <v>1</v>
       </c>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="86" t="s">
         <v>967</v>
       </c>
-      <c r="D9" s="96">
+      <c r="D9" s="88">
         <v>43840</v>
       </c>
-      <c r="E9" s="94">
+      <c r="E9" s="86">
         <v>80000</v>
       </c>
-      <c r="F9" s="94" t="s">
+      <c r="F9" s="86" t="s">
         <v>968</v>
       </c>
-      <c r="G9" s="94">
+      <c r="G9" s="86">
         <v>1</v>
       </c>
       <c r="M9" s="15" t="s">
@@ -7469,22 +7468,22 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="17">
-      <c r="B10" s="94">
+      <c r="B10" s="86">
         <v>2</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="C10" s="86" t="s">
         <v>969</v>
       </c>
-      <c r="D10" s="96">
+      <c r="D10" s="88">
         <v>44336</v>
       </c>
-      <c r="E10" s="94">
+      <c r="E10" s="86">
         <v>70000</v>
       </c>
-      <c r="F10" s="94" t="s">
+      <c r="F10" s="86" t="s">
         <v>970</v>
       </c>
-      <c r="G10" s="94">
+      <c r="G10" s="86">
         <v>1</v>
       </c>
       <c r="M10" s="15" t="s">
@@ -7492,88 +7491,88 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="78" t="s">
         <v>971</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="19">
-      <c r="B15" s="99" t="s">
+      <c r="B15" s="91" t="s">
         <v>972</v>
       </c>
-      <c r="C15" s="99" t="s">
+      <c r="C15" s="91" t="s">
         <v>973</v>
       </c>
-      <c r="D15" s="99" t="s">
+      <c r="D15" s="91" t="s">
         <v>974</v>
       </c>
-      <c r="E15" s="99" t="s">
+      <c r="E15" s="91" t="s">
         <v>975</v>
       </c>
-      <c r="F15" s="99" t="s">
+      <c r="F15" s="91" t="s">
         <v>962</v>
       </c>
-      <c r="G15" s="99" t="s">
+      <c r="G15" s="91" t="s">
         <v>760</v>
       </c>
-      <c r="H15" s="99" t="s">
+      <c r="H15" s="91" t="s">
         <v>976</v>
       </c>
-      <c r="I15" s="99" t="s">
+      <c r="I15" s="91" t="s">
         <v>954</v>
       </c>
-      <c r="L15" s="86" t="s">
+      <c r="L15" s="78" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="B16" s="94">
+      <c r="B16" s="86">
         <v>1</v>
       </c>
-      <c r="C16" s="94" t="s">
+      <c r="C16" s="86" t="s">
         <v>977</v>
       </c>
-      <c r="D16" s="94">
+      <c r="D16" s="86">
         <v>3</v>
       </c>
-      <c r="E16" s="97">
+      <c r="E16" s="89">
         <v>0.375</v>
       </c>
-      <c r="F16" s="94">
+      <c r="F16" s="86">
         <v>1</v>
       </c>
-      <c r="G16" s="94">
+      <c r="G16" s="86">
         <v>1</v>
       </c>
-      <c r="H16" s="94">
+      <c r="H16" s="86">
         <v>1</v>
       </c>
-      <c r="I16" s="95">
+      <c r="I16" s="87">
         <v>45839.375</v>
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="B17" s="94">
+      <c r="B17" s="86">
         <v>2</v>
       </c>
-      <c r="C17" s="94" t="s">
+      <c r="C17" s="86" t="s">
         <v>978</v>
       </c>
-      <c r="D17" s="94">
+      <c r="D17" s="86">
         <v>4</v>
       </c>
-      <c r="E17" s="97">
+      <c r="E17" s="89">
         <v>0.45833333333333331</v>
       </c>
-      <c r="F17" s="94">
+      <c r="F17" s="86">
         <v>2</v>
       </c>
-      <c r="G17" s="94">
+      <c r="G17" s="86">
         <v>2</v>
       </c>
-      <c r="H17" s="94">
+      <c r="H17" s="86">
         <v>0</v>
       </c>
-      <c r="I17" s="95">
+      <c r="I17" s="87">
         <v>45839.375</v>
       </c>
     </row>
@@ -7588,66 +7587,66 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="19">
-      <c r="A20" s="86" t="s">
+      <c r="A20" s="78" t="s">
         <v>979</v>
       </c>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="B21" s="99" t="s">
+      <c r="B21" s="91" t="s">
         <v>756</v>
       </c>
-      <c r="C21" s="99" t="s">
+      <c r="C21" s="91" t="s">
         <v>757</v>
       </c>
-      <c r="D21" s="99" t="s">
+      <c r="D21" s="91" t="s">
         <v>758</v>
       </c>
-      <c r="E21" s="99" t="s">
+      <c r="E21" s="91" t="s">
         <v>759</v>
       </c>
-      <c r="F21" s="99" t="s">
+      <c r="F21" s="91" t="s">
         <v>980</v>
       </c>
-      <c r="G21" s="99" t="s">
+      <c r="G21" s="91" t="s">
         <v>981</v>
       </c>
-      <c r="H21" s="99" t="s">
+      <c r="H21" s="91" t="s">
         <v>982</v>
       </c>
-      <c r="I21" s="99" t="s">
+      <c r="I21" s="91" t="s">
         <v>760</v>
       </c>
-      <c r="J21" s="99" t="s">
+      <c r="J21" s="91" t="s">
         <v>955</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="17">
-      <c r="B22" s="94">
+      <c r="B22" s="86">
         <v>1</v>
       </c>
-      <c r="C22" s="94" t="s">
+      <c r="C22" s="86" t="s">
         <v>761</v>
       </c>
-      <c r="D22" s="94">
+      <c r="D22" s="86">
         <v>22</v>
       </c>
-      <c r="E22" s="94" t="s">
+      <c r="E22" s="86" t="s">
         <v>762</v>
       </c>
-      <c r="F22" s="96">
+      <c r="F22" s="88">
         <v>37681</v>
       </c>
-      <c r="G22" s="96">
+      <c r="G22" s="88">
         <v>44440</v>
       </c>
-      <c r="H22" s="94">
+      <c r="H22" s="86">
         <v>3.6</v>
       </c>
-      <c r="I22" s="94">
+      <c r="I22" s="86">
         <v>1</v>
       </c>
-      <c r="J22" s="94">
+      <c r="J22" s="86">
         <v>1</v>
       </c>
       <c r="M22" s="15" t="s">
@@ -7655,31 +7654,31 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="17">
-      <c r="B23" s="94">
+      <c r="B23" s="86">
         <v>2</v>
       </c>
-      <c r="C23" s="94" t="s">
+      <c r="C23" s="86" t="s">
         <v>763</v>
       </c>
-      <c r="D23" s="94">
+      <c r="D23" s="86">
         <v>23</v>
       </c>
-      <c r="E23" s="94" t="s">
+      <c r="E23" s="86" t="s">
         <v>764</v>
       </c>
-      <c r="F23" s="96">
+      <c r="F23" s="88">
         <v>37448</v>
       </c>
-      <c r="G23" s="96">
+      <c r="G23" s="88">
         <v>44075</v>
       </c>
-      <c r="H23" s="94">
+      <c r="H23" s="86">
         <v>3.2</v>
       </c>
-      <c r="I23" s="94">
+      <c r="I23" s="86">
         <v>2</v>
       </c>
-      <c r="J23" s="94">
+      <c r="J23" s="86">
         <v>1</v>
       </c>
       <c r="M23" s="15" t="s">
@@ -7692,91 +7691,91 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="19">
-      <c r="A26" s="93" t="s">
+      <c r="A26" s="85" t="s">
         <v>983</v>
       </c>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="92"/>
-      <c r="B27" s="98" t="s">
+      <c r="A27" s="84"/>
+      <c r="B27" s="90" t="s">
         <v>984</v>
       </c>
-      <c r="C27" s="98" t="s">
+      <c r="C27" s="90" t="s">
         <v>756</v>
       </c>
-      <c r="D27" s="98" t="s">
+      <c r="D27" s="90" t="s">
         <v>972</v>
       </c>
-      <c r="E27" s="98" t="s">
+      <c r="E27" s="90" t="s">
         <v>985</v>
       </c>
-      <c r="F27" s="98" t="s">
+      <c r="F27" s="90" t="s">
         <v>986</v>
       </c>
-      <c r="G27" s="98" t="s">
+      <c r="G27" s="90" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="19">
-      <c r="B28" s="94">
+      <c r="B28" s="86">
         <v>1</v>
       </c>
-      <c r="C28" s="94">
+      <c r="C28" s="86">
         <v>1</v>
       </c>
-      <c r="D28" s="94">
+      <c r="D28" s="86">
         <v>1</v>
       </c>
-      <c r="E28" s="94">
+      <c r="E28" s="86">
         <v>90</v>
       </c>
-      <c r="F28" s="95">
+      <c r="F28" s="87">
         <v>45840.375</v>
       </c>
-      <c r="G28" s="94">
+      <c r="G28" s="86">
         <v>1</v>
       </c>
-      <c r="L28" s="86" t="s">
+      <c r="L28" s="78" t="s">
         <v>1000</v>
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="B29" s="94">
+      <c r="B29" s="86">
         <v>2</v>
       </c>
-      <c r="C29" s="94">
+      <c r="C29" s="86">
         <v>2</v>
       </c>
-      <c r="D29" s="94">
+      <c r="D29" s="86">
         <v>2</v>
       </c>
-      <c r="E29" s="94">
+      <c r="E29" s="86">
         <v>75</v>
       </c>
-      <c r="F29" s="95">
+      <c r="F29" s="87">
         <v>45840.375</v>
       </c>
-      <c r="G29" s="94">
+      <c r="G29" s="86">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:13">
-      <c r="B30" s="94">
+      <c r="B30" s="86">
         <v>3</v>
       </c>
-      <c r="C30" s="94">
+      <c r="C30" s="86">
         <v>1</v>
       </c>
-      <c r="D30" s="94">
+      <c r="D30" s="86">
         <v>2</v>
       </c>
-      <c r="E30" s="94">
+      <c r="E30" s="86">
         <v>65</v>
       </c>
-      <c r="F30" s="95">
+      <c r="F30" s="87">
         <v>45840.375</v>
       </c>
-      <c r="G30" s="94">
+      <c r="G30" s="86">
         <v>1</v>
       </c>
     </row>
@@ -7806,7 +7805,7 @@
       </c>
     </row>
     <row r="41" spans="12:13" ht="19">
-      <c r="L41" s="86" t="s">
+      <c r="L41" s="78" t="s">
         <v>1006</v>
       </c>
     </row>
@@ -7841,7 +7840,7 @@
       </c>
     </row>
     <row r="55" spans="12:13" ht="19">
-      <c r="L55" s="86" t="s">
+      <c r="L55" s="78" t="s">
         <v>1012</v>
       </c>
     </row>
@@ -7881,7 +7880,7 @@
       </c>
     </row>
     <row r="70" spans="12:13" ht="19">
-      <c r="L70" s="86" t="s">
+      <c r="L70" s="78" t="s">
         <v>1017</v>
       </c>
     </row>
@@ -7916,7 +7915,7 @@
       </c>
     </row>
     <row r="84" spans="12:12" ht="19">
-      <c r="L84" s="86" t="s">
+      <c r="L84" s="78" t="s">
         <v>1023</v>
       </c>
     </row>
@@ -7947,7 +7946,7 @@
   </sheetPr>
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="109" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -7965,7 +7964,7 @@
       <c r="A1" s="13" t="s">
         <v>950</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="81" t="s">
         <v>951</v>
       </c>
     </row>
@@ -7973,393 +7972,393 @@
       <c r="A3" s="13"/>
     </row>
     <row r="4" spans="1:7" ht="18">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="79" t="s">
         <v>946</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="G5" s="88" t="s">
+      <c r="G5" s="80" t="s">
         <v>888</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="82" t="s">
         <v>873</v>
       </c>
       <c r="C6" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="88" t="s">
+      <c r="G6" s="80" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="83" t="s">
         <v>874</v>
       </c>
-      <c r="C7" s="91" t="s">
+      <c r="C7" s="83" t="s">
         <v>875</v>
       </c>
-      <c r="D7" s="91" t="s">
+      <c r="D7" s="83" t="s">
         <v>876</v>
       </c>
-      <c r="G7" s="88" t="s">
+      <c r="G7" s="80" t="s">
         <v>890</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="83" t="s">
         <v>877</v>
       </c>
-      <c r="C8" s="91" t="s">
+      <c r="C8" s="83" t="s">
         <v>878</v>
       </c>
-      <c r="D8" s="91" t="s">
+      <c r="D8" s="83" t="s">
         <v>879</v>
       </c>
-      <c r="G8" s="88" t="s">
+      <c r="G8" s="80" t="s">
         <v>891</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18">
-      <c r="A9" s="87"/>
-      <c r="B9" s="91" t="s">
+      <c r="A9" s="79"/>
+      <c r="B9" s="83" t="s">
         <v>880</v>
       </c>
-      <c r="C9" s="91" t="s">
+      <c r="C9" s="83" t="s">
         <v>881</v>
       </c>
-      <c r="D9" s="91" t="s">
+      <c r="D9" s="83" t="s">
         <v>882</v>
       </c>
-      <c r="G9" s="88" t="s">
+      <c r="G9" s="80" t="s">
         <v>892</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="83" t="s">
         <v>883</v>
       </c>
-      <c r="C10" s="91" t="s">
+      <c r="C10" s="83" t="s">
         <v>884</v>
       </c>
-      <c r="D10" s="91" t="s">
+      <c r="D10" s="83" t="s">
         <v>885</v>
       </c>
-      <c r="G10" s="88" t="s">
+      <c r="G10" s="80" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18">
-      <c r="A11" s="87"/>
-      <c r="B11" s="91" t="s">
+      <c r="A11" s="79"/>
+      <c r="B11" s="83" t="s">
         <v>886</v>
       </c>
-      <c r="C11" s="91" t="s">
+      <c r="C11" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="D11" s="91" t="s">
+      <c r="D11" s="83" t="s">
         <v>887</v>
       </c>
-      <c r="G11" s="88" t="s">
+      <c r="G11" s="80" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="79" t="s">
         <v>947</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="G17" s="88" t="s">
+      <c r="G17" s="80" t="s">
         <v>903</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="B18" s="90" t="s">
+      <c r="B18" s="82" t="s">
         <v>873</v>
       </c>
-      <c r="C18" s="90" t="s">
+      <c r="C18" s="82" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="90" t="s">
+      <c r="D18" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="G18" s="88" t="s">
+      <c r="G18" s="80" t="s">
         <v>904</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="83" t="s">
         <v>894</v>
       </c>
-      <c r="C19" s="91" t="s">
+      <c r="C19" s="83" t="s">
         <v>875</v>
       </c>
-      <c r="D19" s="91" t="s">
+      <c r="D19" s="83" t="s">
         <v>895</v>
       </c>
-      <c r="G19" s="88" t="s">
+      <c r="G19" s="80" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="B20" s="91" t="s">
+      <c r="B20" s="83" t="s">
         <v>896</v>
       </c>
-      <c r="C20" s="91" t="s">
+      <c r="C20" s="83" t="s">
         <v>878</v>
       </c>
-      <c r="D20" s="91" t="s">
+      <c r="D20" s="83" t="s">
         <v>897</v>
       </c>
-      <c r="G20" s="88" t="s">
+      <c r="G20" s="80" t="s">
         <v>906</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="B21" s="91" t="s">
+      <c r="B21" s="83" t="s">
         <v>898</v>
       </c>
-      <c r="C21" s="91" t="s">
+      <c r="C21" s="83" t="s">
         <v>881</v>
       </c>
-      <c r="D21" s="91" t="s">
+      <c r="D21" s="83" t="s">
         <v>899</v>
       </c>
-      <c r="G21" s="88" t="s">
+      <c r="G21" s="80" t="s">
         <v>907</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="83" t="s">
         <v>900</v>
       </c>
-      <c r="C22" s="91" t="s">
+      <c r="C22" s="83" t="s">
         <v>901</v>
       </c>
-      <c r="D22" s="91" t="s">
+      <c r="D22" s="83" t="s">
         <v>902</v>
       </c>
-      <c r="G22" s="88" t="s">
+      <c r="G22" s="80" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="79" t="s">
         <v>948</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18">
-      <c r="A28" s="87"/>
-      <c r="B28" s="90" t="s">
+      <c r="A28" s="79"/>
+      <c r="B28" s="82" t="s">
         <v>873</v>
       </c>
-      <c r="C28" s="90" t="s">
+      <c r="C28" s="82" t="s">
         <v>168</v>
       </c>
-      <c r="D28" s="90" t="s">
+      <c r="D28" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="G28" s="88" t="s">
+      <c r="G28" s="80" t="s">
         <v>923</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="B29" s="91" t="s">
+      <c r="B29" s="83" t="s">
         <v>908</v>
       </c>
-      <c r="C29" s="91" t="s">
+      <c r="C29" s="83" t="s">
         <v>875</v>
       </c>
-      <c r="D29" s="91" t="s">
+      <c r="D29" s="83" t="s">
         <v>909</v>
       </c>
-      <c r="G29" s="88" t="s">
+      <c r="G29" s="80" t="s">
         <v>924</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18">
-      <c r="A30" s="87"/>
-      <c r="B30" s="91" t="s">
+      <c r="A30" s="79"/>
+      <c r="B30" s="83" t="s">
         <v>874</v>
       </c>
-      <c r="C30" s="91" t="s">
+      <c r="C30" s="83" t="s">
         <v>910</v>
       </c>
-      <c r="D30" s="91" t="s">
+      <c r="D30" s="83" t="s">
         <v>911</v>
       </c>
-      <c r="G30" s="88" t="s">
+      <c r="G30" s="80" t="s">
         <v>925</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="B31" s="91" t="s">
+      <c r="B31" s="83" t="s">
         <v>894</v>
       </c>
-      <c r="C31" s="91" t="s">
+      <c r="C31" s="83" t="s">
         <v>910</v>
       </c>
-      <c r="D31" s="91" t="s">
+      <c r="D31" s="83" t="s">
         <v>912</v>
       </c>
-      <c r="G31" s="88" t="s">
+      <c r="G31" s="80" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="B32" s="91" t="s">
+      <c r="B32" s="83" t="s">
         <v>913</v>
       </c>
-      <c r="C32" s="91" t="s">
+      <c r="C32" s="83" t="s">
         <v>901</v>
       </c>
-      <c r="D32" s="91" t="s">
+      <c r="D32" s="83" t="s">
         <v>914</v>
       </c>
-      <c r="G32" s="88" t="s">
+      <c r="G32" s="80" t="s">
         <v>927</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="B33" s="91" t="s">
+      <c r="B33" s="83" t="s">
         <v>915</v>
       </c>
-      <c r="C33" s="91" t="s">
+      <c r="C33" s="83" t="s">
         <v>884</v>
       </c>
-      <c r="D33" s="91" t="s">
+      <c r="D33" s="83" t="s">
         <v>916</v>
       </c>
-      <c r="G33" s="88" t="s">
+      <c r="G33" s="80" t="s">
         <v>928</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="B34" s="91" t="s">
+      <c r="B34" s="83" t="s">
         <v>917</v>
       </c>
-      <c r="C34" s="91" t="s">
+      <c r="C34" s="83" t="s">
         <v>884</v>
       </c>
-      <c r="D34" s="91" t="s">
+      <c r="D34" s="83" t="s">
         <v>918</v>
       </c>
-      <c r="G34" s="88" t="s">
+      <c r="G34" s="80" t="s">
         <v>929</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="B35" s="91" t="s">
+      <c r="B35" s="83" t="s">
         <v>919</v>
       </c>
-      <c r="C35" s="91" t="s">
+      <c r="C35" s="83" t="s">
         <v>884</v>
       </c>
-      <c r="D35" s="91" t="s">
+      <c r="D35" s="83" t="s">
         <v>920</v>
       </c>
-      <c r="G35" s="88" t="s">
+      <c r="G35" s="80" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="B36" s="91" t="s">
+      <c r="B36" s="83" t="s">
         <v>921</v>
       </c>
-      <c r="C36" s="91" t="s">
+      <c r="C36" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="D36" s="91" t="s">
+      <c r="D36" s="83" t="s">
         <v>922</v>
       </c>
-      <c r="G36" s="88" t="s">
+      <c r="G36" s="80" t="s">
         <v>931</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="G37" s="88" t="s">
+      <c r="G37" s="80" t="s">
         <v>932</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="G38" s="88" t="s">
+      <c r="G38" s="80" t="s">
         <v>933</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="G39" s="88" t="s">
+      <c r="G39" s="80" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18">
-      <c r="A42" s="87" t="s">
+      <c r="A42" s="79" t="s">
         <v>949</v>
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="G43" s="88" t="s">
+      <c r="G43" s="80" t="s">
         <v>937</v>
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="B44" s="90" t="s">
+      <c r="B44" s="82" t="s">
         <v>873</v>
       </c>
-      <c r="C44" s="90" t="s">
+      <c r="C44" s="82" t="s">
         <v>168</v>
       </c>
-      <c r="D44" s="90" t="s">
+      <c r="D44" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="G44" s="88" t="s">
+      <c r="G44" s="80" t="s">
         <v>925</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="B45" s="91" t="s">
+      <c r="B45" s="83" t="s">
         <v>874</v>
       </c>
-      <c r="C45" s="91" t="s">
+      <c r="C45" s="83" t="s">
         <v>910</v>
       </c>
-      <c r="D45" s="91" t="s">
+      <c r="D45" s="83" t="s">
         <v>934</v>
       </c>
-      <c r="G45" s="88" t="s">
+      <c r="G45" s="80" t="s">
         <v>938</v>
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="B46" s="91" t="s">
+      <c r="B46" s="83" t="s">
         <v>935</v>
       </c>
-      <c r="C46" s="91" t="s">
+      <c r="C46" s="83" t="s">
         <v>910</v>
       </c>
-      <c r="D46" s="91" t="s">
+      <c r="D46" s="83" t="s">
         <v>936</v>
       </c>
-      <c r="G46" s="88" t="s">
+      <c r="G46" s="80" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="G47" s="88" t="s">
+      <c r="G47" s="80" t="s">
         <v>932</v>
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="G48" s="88" t="s">
+      <c r="G48" s="80" t="s">
         <v>940</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="G49" s="88" t="s">
+      <c r="G49" s="80" t="s">
         <v>100</v>
       </c>
     </row>
@@ -8369,44 +8368,44 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="18">
-      <c r="B53" s="100" t="s">
+      <c r="B53" s="92" t="s">
         <v>942</v>
       </c>
-      <c r="C53" s="100"/>
+      <c r="C53" s="92"/>
     </row>
     <row r="54" spans="1:7" ht="18">
-      <c r="B54" s="100"/>
-      <c r="C54" s="100"/>
+      <c r="B54" s="92"/>
+      <c r="C54" s="92"/>
     </row>
     <row r="55" spans="1:7" ht="18">
-      <c r="B55" s="100"/>
-      <c r="C55" s="100" t="s">
+      <c r="B55" s="92"/>
+      <c r="C55" s="92" t="s">
         <v>943</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="18">
-      <c r="B56" s="100"/>
-      <c r="C56" s="100"/>
+      <c r="B56" s="92"/>
+      <c r="C56" s="92"/>
     </row>
     <row r="57" spans="1:7" ht="18">
-      <c r="B57" s="100"/>
-      <c r="C57" s="100" t="s">
+      <c r="B57" s="92"/>
+      <c r="C57" s="92" t="s">
         <v>944</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="18">
-      <c r="B58" s="100"/>
-      <c r="C58" s="100"/>
+      <c r="B58" s="92"/>
+      <c r="C58" s="92"/>
     </row>
     <row r="59" spans="1:7" ht="18">
-      <c r="B59" s="100"/>
-      <c r="C59" s="100" t="s">
+      <c r="B59" s="92"/>
+      <c r="C59" s="92" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18">
-      <c r="B60" s="100"/>
-      <c r="C60" s="100"/>
+      <c r="B60" s="92"/>
+      <c r="C60" s="92"/>
     </row>
     <row r="75" spans="1:1" ht="23">
       <c r="A75" s="13"/>
@@ -8675,10 +8674,10 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="C46" s="79" t="s">
+      <c r="C46" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="D46" s="79"/>
+      <c r="D46" s="107"/>
     </row>
     <row r="47" spans="1:4">
       <c r="B47" s="22" t="s">
@@ -8898,7 +8897,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="B16" s="83" t="s">
+      <c r="B16" s="111" t="s">
         <v>200</v>
       </c>
       <c r="C16" s="26" t="s">
@@ -8912,7 +8911,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="B17" s="84"/>
+      <c r="B17" s="112"/>
       <c r="C17" s="58" t="s">
         <v>485</v>
       </c>
@@ -8924,7 +8923,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="111" t="s">
         <v>205</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -8938,7 +8937,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="B19" s="84"/>
+      <c r="B19" s="112"/>
       <c r="C19" s="26" t="s">
         <v>209</v>
       </c>
@@ -8950,7 +8949,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="111" t="s">
         <v>212</v>
       </c>
       <c r="C20" s="26" t="s">
@@ -8964,7 +8963,7 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="B21" s="84"/>
+      <c r="B21" s="112"/>
       <c r="C21" s="26" t="s">
         <v>216</v>
       </c>
@@ -9004,7 +9003,7 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="111" t="s">
         <v>227</v>
       </c>
       <c r="C24" s="26" t="s">
@@ -9018,7 +9017,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="B25" s="85"/>
+      <c r="B25" s="113"/>
       <c r="C25" s="26" t="s">
         <v>229</v>
       </c>
@@ -9030,7 +9029,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="B26" s="84"/>
+      <c r="B26" s="112"/>
       <c r="C26" s="26" t="s">
         <v>232</v>
       </c>
@@ -9070,7 +9069,7 @@
       </c>
     </row>
     <row r="35" spans="2:12">
-      <c r="B35" s="80" t="s">
+      <c r="B35" s="108" t="s">
         <v>240</v>
       </c>
       <c r="C35" s="26" t="s">
@@ -9084,7 +9083,7 @@
       </c>
     </row>
     <row r="36" spans="2:12">
-      <c r="B36" s="81"/>
+      <c r="B36" s="109"/>
       <c r="C36" s="26" t="s">
         <v>243</v>
       </c>
@@ -9096,7 +9095,7 @@
       </c>
     </row>
     <row r="37" spans="2:12">
-      <c r="B37" s="81"/>
+      <c r="B37" s="109"/>
       <c r="C37" s="26" t="s">
         <v>604</v>
       </c>
@@ -9108,7 +9107,7 @@
       </c>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" s="81"/>
+      <c r="B38" s="109"/>
       <c r="C38" s="26" t="s">
         <v>248</v>
       </c>
@@ -9120,7 +9119,7 @@
       </c>
     </row>
     <row r="39" spans="2:12">
-      <c r="B39" s="81"/>
+      <c r="B39" s="109"/>
       <c r="C39" s="26" t="s">
         <v>250</v>
       </c>
@@ -9132,7 +9131,7 @@
       </c>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="82"/>
+      <c r="B40" s="110"/>
       <c r="C40" s="26" t="s">
         <v>252</v>
       </c>
@@ -9144,7 +9143,7 @@
       </c>
     </row>
     <row r="41" spans="2:12">
-      <c r="B41" s="80" t="s">
+      <c r="B41" s="108" t="s">
         <v>255</v>
       </c>
       <c r="C41" s="26" t="s">
@@ -9158,7 +9157,7 @@
       </c>
     </row>
     <row r="42" spans="2:12">
-      <c r="B42" s="81"/>
+      <c r="B42" s="109"/>
       <c r="C42" s="26" t="s">
         <v>259</v>
       </c>
@@ -9170,7 +9169,7 @@
       </c>
     </row>
     <row r="43" spans="2:12">
-      <c r="B43" s="81"/>
+      <c r="B43" s="109"/>
       <c r="C43" s="59" t="s">
         <v>606</v>
       </c>
@@ -9185,7 +9184,7 @@
       </c>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="81"/>
+      <c r="B44" s="109"/>
       <c r="C44" s="26" t="s">
         <v>605</v>
       </c>
@@ -9197,7 +9196,7 @@
       </c>
     </row>
     <row r="45" spans="2:12">
-      <c r="B45" s="81"/>
+      <c r="B45" s="109"/>
       <c r="C45" s="26" t="s">
         <v>264</v>
       </c>
@@ -9212,7 +9211,7 @@
       </c>
     </row>
     <row r="46" spans="2:12">
-      <c r="B46" s="82"/>
+      <c r="B46" s="110"/>
       <c r="C46" s="26" t="s">
         <v>266</v>
       </c>
@@ -9225,7 +9224,7 @@
       <c r="L46" s="46"/>
     </row>
     <row r="47" spans="2:12">
-      <c r="B47" s="80" t="s">
+      <c r="B47" s="108" t="s">
         <v>268</v>
       </c>
       <c r="C47" s="26" t="s">
@@ -9242,7 +9241,7 @@
       </c>
     </row>
     <row r="48" spans="2:12">
-      <c r="B48" s="81"/>
+      <c r="B48" s="109"/>
       <c r="C48" s="26" t="s">
         <v>272</v>
       </c>
@@ -9255,7 +9254,7 @@
       <c r="L48" s="46"/>
     </row>
     <row r="49" spans="2:12">
-      <c r="B49" s="81"/>
+      <c r="B49" s="109"/>
       <c r="C49" s="26" t="s">
         <v>275</v>
       </c>
@@ -9270,7 +9269,7 @@
       </c>
     </row>
     <row r="50" spans="2:12">
-      <c r="B50" s="81"/>
+      <c r="B50" s="109"/>
       <c r="C50" s="26" t="s">
         <v>278</v>
       </c>
@@ -9283,7 +9282,7 @@
       <c r="L50" s="46"/>
     </row>
     <row r="51" spans="2:12">
-      <c r="B51" s="81"/>
+      <c r="B51" s="109"/>
       <c r="C51" s="26" t="s">
         <v>281</v>
       </c>
@@ -9298,7 +9297,7 @@
       </c>
     </row>
     <row r="52" spans="2:12">
-      <c r="B52" s="82"/>
+      <c r="B52" s="110"/>
       <c r="C52" s="26" t="s">
         <v>284</v>
       </c>
@@ -9310,7 +9309,7 @@
       </c>
     </row>
     <row r="53" spans="2:12">
-      <c r="B53" s="80" t="s">
+      <c r="B53" s="108" t="s">
         <v>287</v>
       </c>
       <c r="C53" s="48" t="s">
@@ -9324,7 +9323,7 @@
       </c>
     </row>
     <row r="54" spans="2:12">
-      <c r="B54" s="81"/>
+      <c r="B54" s="109"/>
       <c r="C54" s="48" t="s">
         <v>291</v>
       </c>
@@ -9336,7 +9335,7 @@
       </c>
     </row>
     <row r="55" spans="2:12">
-      <c r="B55" s="81"/>
+      <c r="B55" s="109"/>
       <c r="C55" s="48" t="s">
         <v>294</v>
       </c>
@@ -9348,7 +9347,7 @@
       </c>
     </row>
     <row r="56" spans="2:12">
-      <c r="B56" s="81"/>
+      <c r="B56" s="109"/>
       <c r="C56" s="48" t="s">
         <v>297</v>
       </c>
@@ -9360,7 +9359,7 @@
       </c>
     </row>
     <row r="57" spans="2:12">
-      <c r="B57" s="82"/>
+      <c r="B57" s="110"/>
       <c r="C57" s="48" t="s">
         <v>300</v>
       </c>
@@ -9372,7 +9371,7 @@
       </c>
     </row>
     <row r="58" spans="2:12">
-      <c r="B58" s="80" t="s">
+      <c r="B58" s="108" t="s">
         <v>303</v>
       </c>
       <c r="C58" s="26" t="s">
@@ -9386,7 +9385,7 @@
       </c>
     </row>
     <row r="59" spans="2:12">
-      <c r="B59" s="81"/>
+      <c r="B59" s="109"/>
       <c r="C59" s="26" t="s">
         <v>307</v>
       </c>
@@ -9398,7 +9397,7 @@
       </c>
     </row>
     <row r="60" spans="2:12">
-      <c r="B60" s="81"/>
+      <c r="B60" s="109"/>
       <c r="C60" s="26" t="s">
         <v>310</v>
       </c>
@@ -9410,7 +9409,7 @@
       </c>
     </row>
     <row r="61" spans="2:12">
-      <c r="B61" s="82"/>
+      <c r="B61" s="110"/>
       <c r="C61" s="26" t="s">
         <v>313</v>
       </c>
@@ -12351,9 +12350,9 @@
   </sheetPr>
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="31.83203125" defaultRowHeight="24"/>
@@ -12363,7 +12362,7 @@
     <col min="3" max="3" width="17.33203125" style="63" customWidth="1"/>
     <col min="4" max="4" width="18" style="63" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" style="63" customWidth="1"/>
-    <col min="6" max="6" width="27" style="63" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" style="63" customWidth="1"/>
     <col min="7" max="7" width="54.5" style="63" customWidth="1"/>
     <col min="8" max="8" width="31.83203125" style="66"/>
     <col min="9" max="16384" width="31.83203125" style="63"/>
@@ -12636,7 +12635,7 @@
       <c r="E13" s="64">
         <v>1</v>
       </c>
-      <c r="G13" s="109" t="s">
+      <c r="G13" s="100" t="s">
         <v>816</v>
       </c>
     </row>
@@ -12986,7 +12985,7 @@
       <c r="E31" s="64">
         <v>1</v>
       </c>
-      <c r="G31" s="112" t="s">
+      <c r="G31" s="103" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -13007,7 +13006,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="24"/>
-      <c r="H32" s="110" t="s">
+      <c r="H32" s="101" t="s">
         <v>824</v>
       </c>
     </row>
@@ -13028,7 +13027,7 @@
         <v>2</v>
       </c>
       <c r="G33" s="24"/>
-      <c r="H33" s="110" t="s">
+      <c r="H33" s="101" t="s">
         <v>630</v>
       </c>
     </row>
@@ -13049,7 +13048,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="22"/>
-      <c r="H34" s="110" t="s">
+      <c r="H34" s="101" t="s">
         <v>825</v>
       </c>
     </row>
@@ -13070,7 +13069,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="24"/>
-      <c r="H35" s="110" t="s">
+      <c r="H35" s="101" t="s">
         <v>1101</v>
       </c>
     </row>
@@ -13088,7 +13087,7 @@
         <v>764</v>
       </c>
       <c r="E36" s="64"/>
-      <c r="H36" s="111"/>
+      <c r="H36" s="102"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="64">
@@ -13107,7 +13106,7 @@
         <v>2</v>
       </c>
       <c r="G37" s="24"/>
-      <c r="H37" s="111"/>
+      <c r="H37" s="102"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="64">
@@ -13504,7 +13503,7 @@
         <v>291</v>
       </c>
       <c r="G79" s="21"/>
-      <c r="H79" s="113" t="s">
+      <c r="H79" s="104" t="s">
         <v>847</v>
       </c>
     </row>
@@ -13512,7 +13511,7 @@
       <c r="F80" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="H80" s="113" t="s">
+      <c r="H80" s="104" t="s">
         <v>630</v>
       </c>
     </row>
@@ -13520,7 +13519,7 @@
       <c r="F81" s="48" t="s">
         <v>297</v>
       </c>
-      <c r="H81" s="113" t="s">
+      <c r="H81" s="104" t="s">
         <v>848</v>
       </c>
     </row>
@@ -13528,12 +13527,12 @@
       <c r="F82" s="48" t="s">
         <v>300</v>
       </c>
-      <c r="H82" s="113" t="s">
+      <c r="H82" s="104" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="83" spans="6:8">
-      <c r="H83" s="114"/>
+      <c r="H83" s="105"/>
     </row>
     <row r="84" spans="6:8">
       <c r="G84" s="21"/>
@@ -13809,7 +13808,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A32"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14371,13 +14370,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53120742-3F66-A846-9F6C-4E1D1E46BC73}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="102"/>
+    <col min="1" max="1" width="10.83203125" style="94"/>
     <col min="2" max="2" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -14423,7 +14420,7 @@
       <c r="C9" s="46" t="s">
         <v>1029</v>
       </c>
-      <c r="H9" s="103" t="s">
+      <c r="H9" s="95" t="s">
         <v>1056</v>
       </c>
     </row>
@@ -14431,7 +14428,7 @@
       <c r="C10" s="46" t="s">
         <v>1030</v>
       </c>
-      <c r="H10" s="103" t="s">
+      <c r="H10" s="95" t="s">
         <v>1057</v>
       </c>
     </row>
@@ -14439,7 +14436,7 @@
       <c r="C11" s="46" t="s">
         <v>1031</v>
       </c>
-      <c r="H11" s="103" t="s">
+      <c r="H11" s="95" t="s">
         <v>1058</v>
       </c>
     </row>
@@ -14447,7 +14444,7 @@
       <c r="C12" s="46" t="s">
         <v>1032</v>
       </c>
-      <c r="H12" s="103" t="s">
+      <c r="H12" s="95" t="s">
         <v>1059</v>
       </c>
     </row>
@@ -14479,7 +14476,7 @@
       <c r="C21" s="46" t="s">
         <v>1029</v>
       </c>
-      <c r="H21" s="103" t="s">
+      <c r="H21" s="95" t="s">
         <v>1060</v>
       </c>
     </row>
@@ -14543,7 +14540,7 @@
       <c r="C33" s="46" t="s">
         <v>1029</v>
       </c>
-      <c r="H33" s="103" t="s">
+      <c r="H33" s="95" t="s">
         <v>1060</v>
       </c>
     </row>
@@ -14568,7 +14565,7 @@
       <c r="B38" s="46"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="101" t="s">
+      <c r="B39" s="93" t="s">
         <v>1035</v>
       </c>
     </row>
@@ -14605,7 +14602,7 @@
       <c r="C47" s="46" t="s">
         <v>1029</v>
       </c>
-      <c r="H47" s="103" t="s">
+      <c r="H47" s="95" t="s">
         <v>1061</v>
       </c>
     </row>
@@ -14630,7 +14627,7 @@
       <c r="B52" s="46"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="B53" s="101" t="s">
+      <c r="B53" s="93" t="s">
         <v>1037</v>
       </c>
     </row>
@@ -14665,7 +14662,7 @@
       <c r="C61" s="46" t="s">
         <v>1029</v>
       </c>
-      <c r="H61" s="103" t="s">
+      <c r="H61" s="95" t="s">
         <v>1062</v>
       </c>
     </row>
@@ -14710,7 +14707,7 @@
       <c r="C72" s="46" t="s">
         <v>1040</v>
       </c>
-      <c r="H72" s="103" t="s">
+      <c r="H72" s="95" t="s">
         <v>1063</v>
       </c>
     </row>
@@ -14754,97 +14751,97 @@
     </row>
     <row r="141" spans="2:5">
       <c r="B141"/>
-      <c r="C141" s="104" t="s">
+      <c r="C141" s="96" t="s">
         <v>1092</v>
       </c>
-      <c r="D141" s="105" t="s">
+      <c r="D141" s="97" t="s">
         <v>1064</v>
       </c>
-      <c r="E141" s="99" t="s">
+      <c r="E141" s="91" t="s">
         <v>1094</v>
       </c>
     </row>
     <row r="142" spans="2:5">
       <c r="B142"/>
-      <c r="C142" s="94" t="s">
+      <c r="C142" s="86" t="s">
         <v>1084</v>
       </c>
-      <c r="D142" s="94" t="s">
+      <c r="D142" s="86" t="s">
         <v>1066</v>
       </c>
-      <c r="E142" s="94" t="s">
+      <c r="E142" s="86" t="s">
         <v>1078</v>
       </c>
     </row>
     <row r="143" spans="2:5">
       <c r="B143"/>
-      <c r="C143" s="94" t="s">
+      <c r="C143" s="86" t="s">
         <v>1085</v>
       </c>
-      <c r="D143" s="94" t="s">
+      <c r="D143" s="86" t="s">
         <v>1067</v>
       </c>
-      <c r="E143" s="94" t="s">
+      <c r="E143" s="86" t="s">
         <v>1079</v>
       </c>
     </row>
     <row r="144" spans="2:5">
       <c r="B144"/>
-      <c r="C144" s="94" t="s">
+      <c r="C144" s="86" t="s">
         <v>1086</v>
       </c>
-      <c r="D144" s="94" t="s">
+      <c r="D144" s="86" t="s">
         <v>1068</v>
       </c>
-      <c r="E144" s="94" t="s">
+      <c r="E144" s="86" t="s">
         <v>1080</v>
       </c>
     </row>
     <row r="145" spans="2:5">
       <c r="B145"/>
-      <c r="C145" s="94" t="s">
+      <c r="C145" s="86" t="s">
         <v>1087</v>
       </c>
-      <c r="D145" s="94" t="s">
+      <c r="D145" s="86" t="s">
         <v>1069</v>
       </c>
-      <c r="E145" s="94" t="s">
+      <c r="E145" s="86" t="s">
         <v>1081</v>
       </c>
     </row>
     <row r="146" spans="2:5">
       <c r="B146"/>
-      <c r="C146" s="94" t="s">
+      <c r="C146" s="86" t="s">
         <v>1088</v>
       </c>
-      <c r="D146" s="94" t="s">
+      <c r="D146" s="86" t="s">
         <v>1070</v>
       </c>
-      <c r="E146" s="94" t="s">
+      <c r="E146" s="86" t="s">
         <v>1082</v>
       </c>
     </row>
     <row r="147" spans="2:5">
       <c r="B147"/>
-      <c r="C147" s="94" t="s">
+      <c r="C147" s="86" t="s">
         <v>1089</v>
       </c>
-      <c r="D147" s="94" t="s">
+      <c r="D147" s="86" t="s">
         <v>1071</v>
       </c>
-      <c r="E147" s="94" t="s">
+      <c r="E147" s="86" t="s">
         <v>1083</v>
       </c>
     </row>
     <row r="148" spans="2:5">
       <c r="B148"/>
-      <c r="C148" s="107" t="s">
+      <c r="C148" s="98" t="s">
         <v>1096</v>
       </c>
-      <c r="D148" s="106" t="s">
+      <c r="D148" s="86" t="s">
         <v>1097</v>
       </c>
-      <c r="E148" s="108" t="s">
+      <c r="E148" s="99" t="s">
         <v>68</v>
       </c>
     </row>
@@ -14858,97 +14855,97 @@
     </row>
     <row r="151" spans="2:5">
       <c r="B151"/>
-      <c r="C151" s="104" t="s">
+      <c r="C151" s="96" t="s">
         <v>1093</v>
       </c>
-      <c r="D151" s="105" t="s">
+      <c r="D151" s="97" t="s">
         <v>1065</v>
       </c>
-      <c r="E151" s="99" t="s">
+      <c r="E151" s="91" t="s">
         <v>1095</v>
       </c>
     </row>
     <row r="152" spans="2:5">
       <c r="B152"/>
-      <c r="C152" s="94" t="s">
+      <c r="C152" s="86" t="s">
         <v>1078</v>
       </c>
-      <c r="D152" s="94" t="s">
+      <c r="D152" s="86" t="s">
         <v>1072</v>
       </c>
-      <c r="E152" s="94" t="s">
+      <c r="E152" s="86" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="153" spans="2:5">
       <c r="B153"/>
-      <c r="C153" s="94" t="s">
+      <c r="C153" s="86" t="s">
         <v>1079</v>
       </c>
-      <c r="D153" s="94" t="s">
+      <c r="D153" s="86" t="s">
         <v>1073</v>
       </c>
-      <c r="E153" s="94" t="s">
+      <c r="E153" s="86" t="s">
         <v>1085</v>
       </c>
     </row>
     <row r="154" spans="2:5">
       <c r="B154"/>
-      <c r="C154" s="94" t="s">
+      <c r="C154" s="86" t="s">
         <v>1080</v>
       </c>
-      <c r="D154" s="94" t="s">
+      <c r="D154" s="86" t="s">
         <v>1074</v>
       </c>
-      <c r="E154" s="94" t="s">
+      <c r="E154" s="86" t="s">
         <v>1086</v>
       </c>
     </row>
     <row r="155" spans="2:5">
       <c r="B155"/>
-      <c r="C155" s="94" t="s">
+      <c r="C155" s="86" t="s">
         <v>1081</v>
       </c>
-      <c r="D155" s="94" t="s">
+      <c r="D155" s="86" t="s">
         <v>1075</v>
       </c>
-      <c r="E155" s="94" t="s">
+      <c r="E155" s="86" t="s">
         <v>1087</v>
       </c>
     </row>
     <row r="156" spans="2:5">
       <c r="B156"/>
-      <c r="C156" s="94" t="s">
+      <c r="C156" s="86" t="s">
         <v>1082</v>
       </c>
-      <c r="D156" s="94" t="s">
+      <c r="D156" s="86" t="s">
         <v>1076</v>
       </c>
-      <c r="E156" s="94" t="s">
+      <c r="E156" s="86" t="s">
         <v>1088</v>
       </c>
     </row>
     <row r="157" spans="2:5">
       <c r="B157"/>
-      <c r="C157" s="94" t="s">
+      <c r="C157" s="86" t="s">
         <v>1083</v>
       </c>
-      <c r="D157" s="94" t="s">
+      <c r="D157" s="86" t="s">
         <v>1077</v>
       </c>
-      <c r="E157" s="94" t="s">
+      <c r="E157" s="86" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="158" spans="2:5">
       <c r="B158"/>
-      <c r="C158" s="107" t="s">
+      <c r="C158" s="98" t="s">
         <v>1098</v>
       </c>
-      <c r="D158" s="106" t="s">
+      <c r="D158" s="86" t="s">
         <v>1099</v>
       </c>
-      <c r="E158" s="108" t="s">
+      <c r="E158" s="99" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>